<commit_message>
Actualización edges, añadiendo aristas
Se añaden más aristas para la creación del grafo.
</commit_message>
<xml_diff>
--- a/edges.xlsx
+++ b/edges.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNIVERSIDAD\2021-II\Discretas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3248DD17-65B1-42B4-8A15-DE5737A6DDD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A6D0EFAE-39B8-44F8-BCEF-29BBC5064B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{F796E995-D7BB-471F-95AB-7B8640C3653D}"/>
+    <workbookView xWindow="13464" yWindow="2808" windowWidth="17280" windowHeight="8964" xr2:uid="{F796E995-D7BB-471F-95AB-7B8640C3653D}"/>
   </bookViews>
   <sheets>
     <sheet name="edges" sheetId="1" r:id="rId1"/>
@@ -384,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBDC0AB9-D4A6-4998-9E6A-5BFDDCB189B5}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,10 +452,10 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C6">
-        <v>104.54</v>
+        <v>82.18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -463,13 +463,256 @@
         <v>2</v>
       </c>
       <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>106.83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>88.83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>39</v>
+      </c>
+      <c r="C9">
+        <v>100.35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>40</v>
+      </c>
+      <c r="C10">
+        <v>191.89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>34</v>
+      </c>
+      <c r="C11">
+        <v>247.19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>176.12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>208.72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>145.22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15">
         <v>9</v>
       </c>
-      <c r="C7">
-        <v>82.18</v>
+      <c r="C15">
+        <v>147.52000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>122.61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <v>134.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>31</v>
+      </c>
+      <c r="C18">
+        <v>323.95999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>19</v>
+      </c>
+      <c r="C19">
+        <v>192.28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>12</v>
+      </c>
+      <c r="C20">
+        <v>130.83000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>14</v>
+      </c>
+      <c r="C21">
+        <v>142.30000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>145.69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>62.43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>40</v>
+      </c>
+      <c r="C24">
+        <v>141.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>39</v>
+      </c>
+      <c r="C25">
+        <v>135.25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>41</v>
+      </c>
+      <c r="C26">
+        <v>175.3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <v>43</v>
+      </c>
+      <c r="C27">
+        <v>248.48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>67.61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <v>18</v>
+      </c>
+      <c r="C29">
+        <v>178.63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>